<commit_message>
fix: cd shape : square, hover btn settings,  add readmes, edit workflow
</commit_message>
<xml_diff>
--- a/Jukebox.xlsx
+++ b/Jukebox.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\426\Raspberry\Jukebox-V2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6D13F9D-7BD2-4D91-BEC5-9950A56F6837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73751954-7C21-411C-A0AC-A53187CD5DAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="782" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="782" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Setup Raspberry" sheetId="10" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="338">
   <si>
     <t>Partie App</t>
   </si>
@@ -1151,12 +1151,72 @@
   <si>
     <t>Orange Pi Zero 2</t>
   </si>
+  <si>
+    <t>Se connecter en wifi : sudo raspi-config, system option, WLAN</t>
+  </si>
+  <si>
+    <t>Installer docker</t>
+  </si>
+  <si>
+    <t>1. Assure-toi que ton système est à jour :</t>
+  </si>
+  <si>
+    <t>sudo apt update &amp;&amp; sudo apt upgrade -y</t>
+  </si>
+  <si>
+    <t>2. Installe les dépendances :</t>
+  </si>
+  <si>
+    <t>sudo apt install -y ca-certificates curl gnupg lsb-release</t>
+  </si>
+  <si>
+    <t>3. Ajoute la clé GPG officielle de Docker :</t>
+  </si>
+  <si>
+    <t>sudo mkdir -p /etc/apt/keyrings</t>
+  </si>
+  <si>
+    <t>curl -fsSL https://download.docker.com/linux/debian/gpg | sudo gpg --dearmor -o /etc/apt/keyrings/docker.gpg</t>
+  </si>
+  <si>
+    <t>4. Ajoute le dépôt Docker compatible ARM :</t>
+  </si>
+  <si>
+    <t>echo \</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "deb [arch=armhf signed-by=/etc/apt/keyrings/docker.gpg] https://download.docker.com/linux/debian \</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  $(lsb_release -cs) stable" | \</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  sudo tee /etc/apt/sources.list.d/docker.list &gt; /dev/null</t>
+  </si>
+  <si>
+    <t>5. Met à jour les paquets avec le nouveau dépôt :</t>
+  </si>
+  <si>
+    <t>sudo apt update</t>
+  </si>
+  <si>
+    <t>6. Installe Docker Engine :</t>
+  </si>
+  <si>
+    <t>sudo apt install -y docker-ce docker-ce-cli containerd.io docker-buildx-plugin docker-compose-plugin</t>
+  </si>
+  <si>
+    <t>Eteindre la carte</t>
+  </si>
+  <si>
+    <t>poweroff</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1244,6 +1304,11 @@
     <font>
       <sz val="11"/>
       <name val="Calibri "/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="8">
@@ -1455,7 +1520,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
@@ -1604,6 +1669,15 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2065,220 +2139,302 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5D27CBA-C962-412E-89DF-8B48ECA28584}">
-  <dimension ref="B1:C32"/>
+  <dimension ref="B1:G40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
     <col min="2" max="2" width="43.5546875" customWidth="1"/>
     <col min="3" max="3" width="102.44140625" customWidth="1"/>
+    <col min="6" max="6" width="25.109375" customWidth="1"/>
+    <col min="7" max="7" width="77" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="15" thickBot="1"/>
-    <row r="2" spans="2:3" ht="15" thickBot="1">
-      <c r="B2" s="45" t="s">
+    <row r="1" spans="2:7" ht="15" thickBot="1"/>
+    <row r="2" spans="2:7" ht="15" thickBot="1">
+      <c r="F2" s="45" t="s">
         <v>182</v>
       </c>
-      <c r="C2" s="46" t="s">
+      <c r="G2" s="46" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="3" spans="2:3">
-      <c r="B3" s="41" t="s">
+    <row r="3" spans="2:7">
+      <c r="B3" t="s">
+        <v>336</v>
+      </c>
+      <c r="C3" t="s">
+        <v>337</v>
+      </c>
+      <c r="F3" s="41" t="s">
         <v>183</v>
       </c>
-      <c r="C3" s="44" t="s">
+      <c r="G3" s="44" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="4" spans="2:3">
-      <c r="B4" s="47" t="s">
+    <row r="4" spans="2:7">
+      <c r="F4" s="47" t="s">
         <v>168</v>
       </c>
-      <c r="C4" s="48" t="s">
+      <c r="G4" s="48" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="15">
-      <c r="B5" s="37" t="s">
+    <row r="5" spans="2:7" ht="15">
+      <c r="F5" s="37" t="s">
         <v>172</v>
       </c>
-      <c r="C5" s="38" t="s">
+      <c r="G5" s="38" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="6" spans="2:3" ht="15">
-      <c r="B6" s="39"/>
-      <c r="C6" s="40" t="s">
+    <row r="6" spans="2:7" ht="15">
+      <c r="F6" s="39"/>
+      <c r="G6" s="40" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="15">
-      <c r="B7" s="39"/>
-      <c r="C7" s="40" t="s">
+    <row r="7" spans="2:7" ht="15">
+      <c r="F7" s="39"/>
+      <c r="G7" s="40" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="15">
-      <c r="B8" s="39"/>
-      <c r="C8" s="40" t="s">
+    <row r="8" spans="2:7" ht="15">
+      <c r="F8" s="39"/>
+      <c r="G8" s="40" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="9" spans="2:3" ht="15">
-      <c r="B9" s="39"/>
-      <c r="C9" s="40" t="s">
+    <row r="9" spans="2:7" ht="15">
+      <c r="B9" t="s">
+        <v>318</v>
+      </c>
+      <c r="F9" s="39"/>
+      <c r="G9" s="40" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="10" spans="2:3" ht="15">
-      <c r="B10" s="39"/>
-      <c r="C10" s="40" t="s">
+    <row r="10" spans="2:7" ht="15">
+      <c r="B10" t="s">
+        <v>319</v>
+      </c>
+      <c r="C10" s="67" t="s">
+        <v>320</v>
+      </c>
+      <c r="F10" s="39"/>
+      <c r="G10" s="40" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="11" spans="2:3" ht="15">
-      <c r="B11" s="39"/>
-      <c r="C11" s="40" t="s">
+    <row r="11" spans="2:7" ht="15">
+      <c r="C11" s="69" t="s">
+        <v>321</v>
+      </c>
+      <c r="F11" s="39"/>
+      <c r="G11" s="40" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="15">
-      <c r="B12" s="41"/>
-      <c r="C12" s="42" t="s">
+    <row r="12" spans="2:7" ht="15">
+      <c r="C12" s="67" t="s">
+        <v>322</v>
+      </c>
+      <c r="F12" s="41"/>
+      <c r="G12" s="42" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="13" spans="2:3" ht="15">
-      <c r="B13" s="47" t="s">
+    <row r="13" spans="2:7" ht="15">
+      <c r="C13" s="69" t="s">
+        <v>323</v>
+      </c>
+      <c r="F13" s="47" t="s">
         <v>181</v>
       </c>
-      <c r="C13" s="66" t="s">
+      <c r="G13" s="66" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="14" spans="2:3" ht="15">
-      <c r="B14" s="36" t="s">
+    <row r="14" spans="2:7" ht="15">
+      <c r="C14" s="67" t="s">
+        <v>324</v>
+      </c>
+      <c r="F14" s="36" t="s">
         <v>185</v>
       </c>
-      <c r="C14" s="43" t="s">
+      <c r="G14" s="43" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="15" spans="2:3">
-      <c r="B15" s="49" t="s">
+    <row r="15" spans="2:7">
+      <c r="C15" s="69" t="s">
+        <v>325</v>
+      </c>
+      <c r="F15" s="49" t="s">
         <v>187</v>
       </c>
-      <c r="C15" s="50" t="s">
+      <c r="G15" s="50" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="16" spans="2:3">
-      <c r="B16" s="51" t="s">
+    <row r="16" spans="2:7">
+      <c r="C16" s="69" t="s">
+        <v>326</v>
+      </c>
+      <c r="F16" s="51" t="s">
         <v>315</v>
       </c>
-      <c r="C16" s="52" t="s">
+      <c r="G16" s="52" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="17" spans="2:3">
-      <c r="B17" s="51"/>
-      <c r="C17" s="52" t="s">
+    <row r="17" spans="3:7">
+      <c r="C17" s="67" t="s">
+        <v>327</v>
+      </c>
+      <c r="F17" s="51"/>
+      <c r="G17" s="52" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="18" spans="2:3">
-      <c r="B18" s="51"/>
-      <c r="C18" s="52" t="s">
+    <row r="18" spans="3:7">
+      <c r="C18" s="69" t="s">
+        <v>328</v>
+      </c>
+      <c r="F18" s="51"/>
+      <c r="G18" s="52" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="19" spans="2:3">
-      <c r="B19" s="51"/>
-      <c r="C19" s="52" t="s">
+    <row r="19" spans="3:7">
+      <c r="C19" s="69" t="s">
+        <v>329</v>
+      </c>
+      <c r="F19" s="51"/>
+      <c r="G19" s="52" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="20" spans="2:3">
-      <c r="B20" s="51"/>
-      <c r="C20" s="52" t="s">
+    <row r="20" spans="3:7">
+      <c r="C20" s="69" t="s">
+        <v>330</v>
+      </c>
+      <c r="F20" s="51"/>
+      <c r="G20" s="52" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="21" spans="2:3">
-      <c r="B21" s="51"/>
-      <c r="C21" s="52" t="s">
+    <row r="21" spans="3:7">
+      <c r="C21" s="69" t="s">
+        <v>331</v>
+      </c>
+      <c r="F21" s="51"/>
+      <c r="G21" s="52" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="22" spans="2:3">
-      <c r="B22" s="51"/>
-      <c r="C22" s="52" t="s">
+    <row r="22" spans="3:7">
+      <c r="C22" s="67" t="s">
+        <v>332</v>
+      </c>
+      <c r="F22" s="51"/>
+      <c r="G22" s="52" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="23" spans="2:3">
-      <c r="B23" s="51"/>
-      <c r="C23" s="52" t="s">
+    <row r="23" spans="3:7">
+      <c r="C23" s="69" t="s">
+        <v>333</v>
+      </c>
+      <c r="F23" s="51"/>
+      <c r="G23" s="52" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="24" spans="2:3">
-      <c r="B24" s="51"/>
-      <c r="C24" s="52" t="s">
+    <row r="24" spans="3:7">
+      <c r="C24" s="67" t="s">
+        <v>334</v>
+      </c>
+      <c r="F24" s="51"/>
+      <c r="G24" s="52" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="25" spans="2:3">
-      <c r="B25" s="51"/>
-      <c r="C25" s="52" t="s">
+    <row r="25" spans="3:7">
+      <c r="C25" s="69" t="s">
+        <v>335</v>
+      </c>
+      <c r="F25" s="51"/>
+      <c r="G25" s="52" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="26" spans="2:3">
-      <c r="B26" s="51"/>
-      <c r="C26" s="52" t="s">
+    <row r="26" spans="3:7">
+      <c r="F26" s="51"/>
+      <c r="G26" s="52" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="27" spans="2:3">
-      <c r="B27" s="51"/>
-      <c r="C27" s="52"/>
-    </row>
-    <row r="28" spans="2:3">
-      <c r="B28" s="51"/>
-      <c r="C28" s="52" t="s">
+    <row r="27" spans="3:7">
+      <c r="F27" s="51"/>
+      <c r="G27" s="52"/>
+    </row>
+    <row r="28" spans="3:7">
+      <c r="F28" s="51"/>
+      <c r="G28" s="52" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="29" spans="2:3">
-      <c r="B29" s="51"/>
-      <c r="C29" s="52" t="s">
+    <row r="29" spans="3:7">
+      <c r="F29" s="51"/>
+      <c r="G29" s="52" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="30" spans="2:3">
-      <c r="B30" s="51"/>
-      <c r="C30" s="52" t="s">
+    <row r="30" spans="3:7">
+      <c r="C30" s="32"/>
+      <c r="F30" s="51"/>
+      <c r="G30" s="52" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="31" spans="2:3">
-      <c r="B31" s="51"/>
-      <c r="C31" s="54" t="s">
+    <row r="31" spans="3:7">
+      <c r="F31" s="51"/>
+      <c r="G31" s="54" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="32" spans="2:3">
-      <c r="B32" s="36" t="s">
+    <row r="32" spans="3:7">
+      <c r="C32" s="68"/>
+      <c r="F32" s="36" t="s">
         <v>308</v>
       </c>
-      <c r="C32" s="53" t="s">
+      <c r="G32" s="53" t="s">
         <v>307</v>
       </c>
+    </row>
+    <row r="33" spans="3:3">
+      <c r="C33" s="69"/>
+    </row>
+    <row r="34" spans="3:3">
+      <c r="C34" s="69"/>
+    </row>
+    <row r="36" spans="3:3">
+      <c r="C36" s="32"/>
+    </row>
+    <row r="38" spans="3:3">
+      <c r="C38" s="68"/>
+    </row>
+    <row r="39" spans="3:3">
+      <c r="C39" s="69"/>
+    </row>
+    <row r="40" spans="3:3">
+      <c r="C40" s="69"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2289,7 +2445,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9697DB91-DDD7-46C2-9F18-DA7F9F25DA1F}">
   <dimension ref="B2:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>

</xml_diff>